<commit_message>
Discharging sequence sheet 1 completed , sheet 2 cow sequence table pending , sheet 3 basic items completed
</commit_message>
<xml_diff>
--- a/api/cp-dss-api/gateway/src/main/resources/reports/Vessel_1_Loading_Plan_Template.xlsx
+++ b/api/cp-dss-api/gateway/src/main/resources/reports/Vessel_1_Loading_Plan_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17316" windowHeight="6156" tabRatio="738" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17316" windowHeight="6156" tabRatio="738"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD - 021 pg1" sheetId="27" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <definedName name="SSSN_YESE">#REF!</definedName>
     <definedName name="SSSN_YS">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2188,9 +2188,6 @@
     <t xml:space="preserve">Max.Bend Moment(Fr.No./%)    </t>
   </si>
   <si>
-    <t>LOADING PLAN</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Tolerance +/- %</t>
   </si>
   <si>
@@ -2198,9 +2195,6 @@
   </si>
   <si>
     <t>Time required for Loading (Hrs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     LOADING  SEQUENCE </t>
   </si>
   <si>
     <t>Restricting Load Line Zone for the Voyage:</t>
@@ -3806,6 +3800,12 @@
   </si>
   <si>
     <t>${sheetOne.loadLineZone}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     LOADING  SEQUENCE @ ${sheetOne.portName}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOADING PLAN </t>
   </si>
 </sst>
 </file>
@@ -7311,8 +7311,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AS75"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11:Z11"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.25" customHeight="1"/>
@@ -7370,7 +7370,7 @@
       <c r="J3" s="47"/>
       <c r="K3" s="47"/>
       <c r="L3" s="245" t="s">
-        <v>49</v>
+        <v>584</v>
       </c>
       <c r="M3" s="245"/>
       <c r="N3" s="245"/>
@@ -7395,7 +7395,7 @@
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="251" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E4" s="251"/>
       <c r="F4" s="251"/>
@@ -7428,7 +7428,7 @@
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="324" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="324"/>
       <c r="F5" s="324"/>
@@ -7452,7 +7452,7 @@
         <v>8</v>
       </c>
       <c r="V5" s="268" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="W5" s="268"/>
       <c r="X5" s="268"/>
@@ -7488,7 +7488,7 @@
         <v>8</v>
       </c>
       <c r="V6" s="269" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W6" s="269"/>
       <c r="X6" s="269"/>
@@ -7500,21 +7500,21 @@
     <row r="7" spans="1:32" ht="17.25" customHeight="1">
       <c r="A7" s="57"/>
       <c r="B7" s="58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="252" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="252"/>
       <c r="E7" s="252"/>
       <c r="F7" s="252"/>
       <c r="G7" s="252"/>
       <c r="H7" s="259" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="259"/>
       <c r="J7" s="252" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K7" s="252"/>
       <c r="L7" s="252"/>
@@ -7532,7 +7532,7 @@
         <v>8</v>
       </c>
       <c r="V7" s="269" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="W7" s="269"/>
       <c r="X7" s="269"/>
@@ -7618,7 +7618,7 @@
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
       <c r="P10" s="61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q10" s="62"/>
       <c r="R10" s="62"/>
@@ -7629,7 +7629,7 @@
       <c r="W10" s="61"/>
       <c r="X10" s="61"/>
       <c r="Y10" s="273" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Z10" s="273"/>
       <c r="AB10" s="56"/>
@@ -7655,7 +7655,7 @@
       <c r="N11" s="65"/>
       <c r="O11" s="66"/>
       <c r="P11" s="67" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="67"/>
       <c r="R11" s="67"/>
@@ -7664,7 +7664,7 @@
       <c r="U11" s="67"/>
       <c r="V11" s="68"/>
       <c r="W11" s="274" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="X11" s="274"/>
       <c r="Y11" s="274"/>
@@ -7688,7 +7688,7 @@
       <c r="N12" s="71"/>
       <c r="O12" s="71"/>
       <c r="P12" s="272" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="272"/>
       <c r="R12" s="272"/>
@@ -7750,29 +7750,29 @@
       <c r="A15" s="70"/>
       <c r="B15" s="75"/>
       <c r="C15" s="76" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D15" s="77"/>
       <c r="E15" s="76" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F15" s="78"/>
       <c r="G15" s="223" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H15" s="315"/>
       <c r="I15" s="316"/>
       <c r="J15" s="79" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K15" s="80"/>
       <c r="L15" s="223" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M15" s="315"/>
       <c r="N15" s="316"/>
       <c r="O15" s="79" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P15" s="80"/>
       <c r="Q15" s="81"/>
@@ -7792,35 +7792,35 @@
       <c r="A16" s="84"/>
       <c r="B16" s="85"/>
       <c r="C16" s="247" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="248"/>
       <c r="E16" s="247" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F16" s="249"/>
       <c r="G16" s="247" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H16" s="248"/>
       <c r="I16" s="249"/>
       <c r="J16" s="247" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K16" s="249"/>
       <c r="L16" s="247" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M16" s="248"/>
       <c r="N16" s="249"/>
       <c r="O16" s="247" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P16" s="249"/>
       <c r="Q16" s="85"/>
       <c r="S16" s="71"/>
       <c r="T16" s="275" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="U16" s="275"/>
       <c r="V16" s="275"/>
@@ -7829,7 +7829,7 @@
         <v>8</v>
       </c>
       <c r="Y16" s="277" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Z16" s="277"/>
       <c r="AF16" s="104"/>
@@ -7838,45 +7838,45 @@
       <c r="A17" s="84"/>
       <c r="B17" s="85"/>
       <c r="C17" s="86" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D17" s="87" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E17" s="86" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F17" s="88" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G17" s="220" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H17" s="285" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I17" s="286"/>
       <c r="J17" s="86" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K17" s="87" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L17" s="220" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M17" s="285" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N17" s="286"/>
       <c r="O17" s="86" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="P17" s="89" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q17" s="240" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="S17" s="71"/>
       <c r="T17" s="84"/>
@@ -7898,33 +7898,33 @@
       <c r="A18" s="84"/>
       <c r="B18" s="91"/>
       <c r="C18" s="260" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D18" s="250"/>
       <c r="E18" s="260" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F18" s="261"/>
       <c r="G18" s="260" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H18" s="250"/>
       <c r="I18" s="261"/>
       <c r="J18" s="250" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K18" s="250"/>
       <c r="L18" s="253" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M18" s="254"/>
       <c r="N18" s="255"/>
       <c r="O18" s="250" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P18" s="250"/>
       <c r="Q18" s="276" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="S18" s="71"/>
       <c r="T18" s="270"/>
@@ -7942,45 +7942,45 @@
     <row r="19" spans="1:45" s="69" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="84"/>
       <c r="B19" s="240" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C19" s="224" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D19" s="225" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E19" s="224" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F19" s="225" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G19" s="226" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H19" s="262" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I19" s="263"/>
       <c r="J19" s="224" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K19" s="225" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L19" s="224" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M19" s="262" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="N19" s="263"/>
       <c r="O19" s="227" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P19" s="225" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q19" s="276"/>
       <c r="S19" s="71"/>
@@ -7998,48 +7998,48 @@
       <c r="AD19"/>
       <c r="AE19"/>
       <c r="AF19" s="243" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AG19"/>
     </row>
     <row r="20" spans="1:45" s="69" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="84"/>
       <c r="B20" s="246" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C20" s="92" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D20" s="278" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E20" s="279"/>
       <c r="F20" s="280"/>
       <c r="G20" s="221" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H20" s="264" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I20" s="265"/>
       <c r="J20" s="92" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K20" s="94" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L20" s="95" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M20" s="281" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N20" s="282"/>
       <c r="O20" s="95" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="P20" s="93" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q20" s="233"/>
       <c r="S20" s="71"/>
@@ -8054,7 +8054,7 @@
       <c r="AD20"/>
       <c r="AE20"/>
       <c r="AF20" s="283" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="AG20"/>
     </row>
@@ -8062,27 +8062,27 @@
       <c r="A21" s="84"/>
       <c r="B21" s="246"/>
       <c r="C21" s="260" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D21" s="250"/>
       <c r="E21" s="250"/>
       <c r="F21" s="261"/>
       <c r="G21" s="260" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H21" s="250"/>
       <c r="I21" s="261"/>
       <c r="J21" s="253" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K21" s="255"/>
       <c r="L21" s="253" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M21" s="254"/>
       <c r="N21" s="255"/>
       <c r="O21" s="253" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P21" s="255"/>
       <c r="Q21" s="234"/>
@@ -8104,38 +8104,38 @@
       <c r="A22" s="84"/>
       <c r="B22" s="85"/>
       <c r="C22" s="228" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" s="308" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E22" s="308"/>
       <c r="F22" s="309"/>
       <c r="G22" s="229" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H22" s="308" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I22" s="309"/>
       <c r="J22" s="230" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K22" s="231" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L22" s="230" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M22" s="308" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="N22" s="309"/>
       <c r="O22" s="232" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="P22" s="231" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Q22" s="98"/>
       <c r="S22" s="71"/>
@@ -8155,45 +8155,45 @@
       <c r="A23" s="84"/>
       <c r="B23" s="85"/>
       <c r="C23" s="92" t="s">
+        <v>274</v>
+      </c>
+      <c r="D23" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="92" t="s">
         <v>276</v>
       </c>
-      <c r="D23" s="89" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="92" t="s">
-        <v>278</v>
-      </c>
       <c r="F23" s="89" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G23" s="221" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H23" s="264" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I23" s="265"/>
       <c r="J23" s="92" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K23" s="89" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L23" s="221" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M23" s="264" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N23" s="265"/>
       <c r="O23" s="92" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="P23" s="89" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q23" s="240" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="S23" s="71"/>
       <c r="T23" s="73" t="s">
@@ -8216,44 +8216,44 @@
       <c r="A24" s="84"/>
       <c r="B24" s="85"/>
       <c r="C24" s="260" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D24" s="250"/>
       <c r="E24" s="260" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F24" s="250"/>
       <c r="G24" s="256" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H24" s="257"/>
       <c r="I24" s="258"/>
       <c r="J24" s="260" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K24" s="250"/>
       <c r="L24" s="256" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M24" s="257"/>
       <c r="N24" s="258"/>
       <c r="O24" s="260" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P24" s="250"/>
       <c r="Q24" s="276" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="S24" s="71"/>
       <c r="T24" s="288" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="U24" s="288"/>
       <c r="V24" s="288"/>
       <c r="W24" s="288"/>
       <c r="X24" s="82"/>
       <c r="Y24" s="99" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Z24" s="74"/>
       <c r="AD24"/>
@@ -8267,42 +8267,42 @@
       <c r="A25" s="84"/>
       <c r="B25" s="85"/>
       <c r="C25" s="224" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25" s="225" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E25" s="224" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F25" s="225" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G25" s="226" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H25" s="266" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I25" s="267"/>
       <c r="J25" s="224" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K25" s="225" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L25" s="224" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M25" s="310" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N25" s="311"/>
       <c r="O25" s="224" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="P25" s="225" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Q25" s="276"/>
       <c r="S25" s="71"/>
@@ -8324,29 +8324,29 @@
       <c r="A26" s="70"/>
       <c r="B26" s="85"/>
       <c r="C26" s="100" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D26" s="101"/>
       <c r="E26" s="100" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F26" s="102"/>
       <c r="G26" s="222" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H26" s="313"/>
       <c r="I26" s="314"/>
       <c r="J26" s="100" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K26" s="103"/>
       <c r="L26" s="222" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M26" s="313"/>
       <c r="N26" s="314"/>
       <c r="O26" s="76" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="P26" s="103"/>
       <c r="Q26" s="85"/>
@@ -8361,7 +8361,7 @@
       </c>
       <c r="X26" s="82"/>
       <c r="Y26" s="99" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z26" s="71"/>
       <c r="AD26"/>
@@ -8375,36 +8375,36 @@
       <c r="A27" s="84"/>
       <c r="B27" s="75"/>
       <c r="C27" s="247" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D27" s="248"/>
       <c r="E27" s="247" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F27" s="248"/>
       <c r="G27" s="247" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H27" s="248"/>
       <c r="I27" s="249"/>
       <c r="J27" s="247" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K27" s="248"/>
       <c r="L27" s="247" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M27" s="248"/>
       <c r="N27" s="249"/>
       <c r="O27" s="247" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="P27" s="249"/>
       <c r="Q27" s="104"/>
       <c r="R27" s="71"/>
       <c r="S27" s="73"/>
       <c r="T27" s="287" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U27" s="287"/>
       <c r="V27" s="287"/>
@@ -8413,7 +8413,7 @@
       </c>
       <c r="X27" s="82"/>
       <c r="Y27" s="99" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Z27" s="73"/>
       <c r="AD27"/>
@@ -8453,7 +8453,7 @@
       </c>
       <c r="X28" s="73"/>
       <c r="Y28" s="99" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z28" s="73"/>
       <c r="AD28"/>
@@ -8603,7 +8603,7 @@
       <c r="R32" s="112"/>
       <c r="S32" s="112"/>
       <c r="T32" s="289" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U32" s="289"/>
       <c r="V32" s="289"/>
@@ -8612,7 +8612,7 @@
         <v>8</v>
       </c>
       <c r="Y32" s="277" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Z32" s="277"/>
       <c r="AD32"/>
@@ -8636,29 +8636,29 @@
       <c r="A33" s="70"/>
       <c r="B33" s="75"/>
       <c r="C33" s="76" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D33" s="77"/>
       <c r="E33" s="76" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F33" s="78"/>
       <c r="G33" s="223" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H33" s="315"/>
       <c r="I33" s="316"/>
       <c r="J33" s="217" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K33" s="80"/>
       <c r="L33" s="223" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M33" s="315"/>
       <c r="N33" s="316"/>
       <c r="O33" s="217" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="P33" s="80"/>
       <c r="Q33" s="81"/>
@@ -8693,29 +8693,29 @@
       <c r="A34" s="118"/>
       <c r="B34" s="85"/>
       <c r="C34" s="247" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D34" s="249"/>
       <c r="E34" s="247" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F34" s="249"/>
       <c r="G34" s="247" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H34" s="248"/>
       <c r="I34" s="249"/>
       <c r="J34" s="247" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K34" s="249"/>
       <c r="L34" s="247" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M34" s="248"/>
       <c r="N34" s="249"/>
       <c r="O34" s="247" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="P34" s="249"/>
       <c r="Q34" s="85"/>
@@ -8750,45 +8750,45 @@
       <c r="A35" s="118"/>
       <c r="B35" s="85"/>
       <c r="C35" s="220" t="s">
+        <v>295</v>
+      </c>
+      <c r="D35" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="220" t="s">
+        <v>296</v>
+      </c>
+      <c r="F35" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="220" t="s">
         <v>297</v>
       </c>
-      <c r="D35" s="87" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" s="220" t="s">
-        <v>298</v>
-      </c>
-      <c r="F35" s="88" t="s">
-        <v>126</v>
-      </c>
-      <c r="G35" s="220" t="s">
-        <v>299</v>
-      </c>
       <c r="H35" s="285" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I35" s="286"/>
       <c r="J35" s="220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K35" s="87" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L35" s="220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M35" s="285" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N35" s="286"/>
       <c r="O35" s="220" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P35" s="89" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q35" s="244" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="S35" s="116"/>
       <c r="T35" s="117"/>
@@ -8824,33 +8824,33 @@
       <c r="A36" s="118"/>
       <c r="B36" s="85"/>
       <c r="C36" s="260" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D36" s="261"/>
       <c r="E36" s="260" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F36" s="261"/>
       <c r="G36" s="260" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H36" s="250"/>
       <c r="I36" s="261"/>
       <c r="J36" s="260" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K36" s="261"/>
       <c r="L36" s="253" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M36" s="254"/>
       <c r="N36" s="255"/>
       <c r="O36" s="260" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P36" s="261"/>
       <c r="Q36" s="276" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="S36" s="116"/>
       <c r="T36" s="117"/>
@@ -8882,45 +8882,45 @@
     <row r="37" spans="1:45" s="69" customFormat="1" ht="12" customHeight="1">
       <c r="A37" s="118"/>
       <c r="B37" s="242" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C37" s="224" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D37" s="225" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E37" s="224" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F37" s="225" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G37" s="224" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H37" s="262" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I37" s="263"/>
       <c r="J37" s="224" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K37" s="225" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L37" s="224" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M37" s="262" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N37" s="263"/>
       <c r="O37" s="227" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="P37" s="225" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="Q37" s="276"/>
       <c r="S37" s="126"/>
@@ -8936,7 +8936,7 @@
         <v>34</v>
       </c>
       <c r="AF37" s="243" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="AG37" s="237"/>
       <c r="AH37" s="237"/>
@@ -8955,41 +8955,41 @@
     <row r="38" spans="1:45" s="69" customFormat="1" ht="12" customHeight="1">
       <c r="A38" s="118"/>
       <c r="B38" s="246" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C38" s="218" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D38" s="279" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E38" s="279"/>
       <c r="F38" s="312"/>
       <c r="G38" s="221" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H38" s="264" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I38" s="265"/>
       <c r="J38" s="218" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K38" s="219" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L38" s="95" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M38" s="281" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N38" s="282"/>
       <c r="O38" s="95" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P38" s="93" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="Q38" s="233"/>
       <c r="S38" s="116"/>
@@ -9001,7 +9001,7 @@
       <c r="Y38" s="127"/>
       <c r="Z38" s="71"/>
       <c r="AF38" s="283" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="AG38" s="236"/>
       <c r="AH38" s="236"/>
@@ -9021,27 +9021,27 @@
       <c r="A39" s="118"/>
       <c r="B39" s="246"/>
       <c r="C39" s="260" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D39" s="250"/>
       <c r="E39" s="250"/>
       <c r="F39" s="261"/>
       <c r="G39" s="260" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H39" s="250"/>
       <c r="I39" s="261"/>
       <c r="J39" s="253" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K39" s="255"/>
       <c r="L39" s="253" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M39" s="254"/>
       <c r="N39" s="255"/>
       <c r="O39" s="253" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P39" s="255"/>
       <c r="Q39" s="234"/>
@@ -9074,50 +9074,50 @@
       <c r="A40" s="118"/>
       <c r="B40" s="85"/>
       <c r="C40" s="228" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D40" s="308" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E40" s="308"/>
       <c r="F40" s="309"/>
       <c r="G40" s="229" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H40" s="308" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I40" s="309"/>
       <c r="J40" s="230" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K40" s="231" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L40" s="230" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M40" s="308" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N40" s="309"/>
       <c r="O40" s="232" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P40" s="231" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q40" s="98"/>
       <c r="S40" s="65"/>
       <c r="T40" s="288" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="U40" s="288"/>
       <c r="V40" s="288"/>
       <c r="W40" s="288"/>
       <c r="X40" s="82"/>
       <c r="Y40" s="128" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Z40" s="74"/>
       <c r="AF40" s="241"/>
@@ -9139,45 +9139,45 @@
       <c r="A41" s="118"/>
       <c r="B41" s="85"/>
       <c r="C41" s="218" t="s">
+        <v>306</v>
+      </c>
+      <c r="D41" s="89" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="218" t="s">
+        <v>307</v>
+      </c>
+      <c r="F41" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="G41" s="221" t="s">
         <v>308</v>
       </c>
-      <c r="D41" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="E41" s="218" t="s">
-        <v>309</v>
-      </c>
-      <c r="F41" s="89" t="s">
-        <v>134</v>
-      </c>
-      <c r="G41" s="221" t="s">
-        <v>310</v>
-      </c>
       <c r="H41" s="264" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I41" s="265"/>
       <c r="J41" s="218" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K41" s="89" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L41" s="221" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M41" s="264" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N41" s="265"/>
       <c r="O41" s="218" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P41" s="89" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="Q41" s="244" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="S41" s="112"/>
       <c r="T41" s="71"/>
@@ -9206,33 +9206,33 @@
       <c r="A42" s="118"/>
       <c r="B42" s="85"/>
       <c r="C42" s="260" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D42" s="261"/>
       <c r="E42" s="260" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F42" s="261"/>
       <c r="G42" s="256" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H42" s="257"/>
       <c r="I42" s="258"/>
       <c r="J42" s="260" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K42" s="261"/>
       <c r="L42" s="256" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M42" s="257"/>
       <c r="N42" s="258"/>
       <c r="O42" s="260" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P42" s="261"/>
       <c r="Q42" s="276" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="S42" s="71"/>
       <c r="T42" s="287" t="s">
@@ -9245,7 +9245,7 @@
       </c>
       <c r="X42" s="82"/>
       <c r="Y42" s="128" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Z42" s="71"/>
       <c r="AF42" s="104"/>
@@ -9267,47 +9267,47 @@
       <c r="A43" s="118"/>
       <c r="B43" s="85"/>
       <c r="C43" s="224" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D43" s="225" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E43" s="224" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F43" s="225" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G43" s="224" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H43" s="266" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I43" s="267"/>
       <c r="J43" s="224" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K43" s="225" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L43" s="224" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M43" s="262" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N43" s="263"/>
       <c r="O43" s="224" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="P43" s="225" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="Q43" s="276"/>
       <c r="S43" s="71"/>
       <c r="T43" s="287" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U43" s="287"/>
       <c r="V43" s="287"/>
@@ -9316,7 +9316,7 @@
       </c>
       <c r="X43" s="82"/>
       <c r="Y43" s="128" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Z43" s="73"/>
       <c r="AF43" s="104"/>
@@ -9338,29 +9338,29 @@
       <c r="A44" s="129"/>
       <c r="B44" s="85"/>
       <c r="C44" s="100" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D44" s="101"/>
       <c r="E44" s="100" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F44" s="102"/>
       <c r="G44" s="223" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H44" s="315"/>
       <c r="I44" s="316"/>
       <c r="J44" s="100" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K44" s="103"/>
       <c r="L44" s="223" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M44" s="315"/>
       <c r="N44" s="316"/>
       <c r="O44" s="76" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="P44" s="103"/>
       <c r="Q44" s="85"/>
@@ -9375,7 +9375,7 @@
       </c>
       <c r="X44" s="73"/>
       <c r="Y44" s="128" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z44" s="73"/>
       <c r="AC44" s="69" t="s">
@@ -9400,29 +9400,29 @@
       <c r="A45" s="84"/>
       <c r="B45" s="75"/>
       <c r="C45" s="247" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D45" s="249"/>
       <c r="E45" s="247" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F45" s="249"/>
       <c r="G45" s="247" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H45" s="248"/>
       <c r="I45" s="249"/>
       <c r="J45" s="247" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K45" s="249"/>
       <c r="L45" s="247" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="M45" s="248"/>
       <c r="N45" s="249"/>
       <c r="O45" s="247" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P45" s="249"/>
       <c r="Q45" s="104"/>
@@ -9542,13 +9542,13 @@
       <c r="G49" s="139"/>
       <c r="H49" s="140"/>
       <c r="I49" s="323" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J49" s="323"/>
       <c r="K49" s="323"/>
       <c r="L49" s="323"/>
       <c r="M49" s="328" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N49" s="329"/>
       <c r="O49" s="329"/>
@@ -9578,7 +9578,7 @@
       <c r="G50" s="139"/>
       <c r="H50" s="140"/>
       <c r="I50" s="323" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J50" s="323"/>
       <c r="K50" s="323"/>
@@ -9604,7 +9604,7 @@
       <c r="A51" s="135"/>
       <c r="B51" s="141"/>
       <c r="C51" s="139" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D51" s="139"/>
       <c r="E51" s="139"/>
@@ -9612,7 +9612,7 @@
       <c r="G51" s="139"/>
       <c r="H51" s="140"/>
       <c r="I51" s="323" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J51" s="323"/>
       <c r="K51" s="323"/>
@@ -9646,7 +9646,7 @@
       <c r="G52" s="139"/>
       <c r="H52" s="140"/>
       <c r="I52" s="323" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J52" s="323"/>
       <c r="K52" s="323"/>
@@ -9680,7 +9680,7 @@
       <c r="G53" s="139"/>
       <c r="H53" s="140"/>
       <c r="I53" s="323" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J53" s="323"/>
       <c r="K53" s="323"/>
@@ -9714,7 +9714,7 @@
       <c r="G54" s="338"/>
       <c r="H54" s="339"/>
       <c r="I54" s="322" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J54" s="322"/>
       <c r="K54" s="322"/>
@@ -9844,7 +9844,7 @@
         <v>4</v>
       </c>
       <c r="C58" s="143" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D58" s="143"/>
       <c r="E58" s="143"/>
@@ -9943,7 +9943,7 @@
         <v>24</v>
       </c>
       <c r="B61" s="148" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C61" s="148"/>
       <c r="D61" s="148"/>
@@ -9983,7 +9983,7 @@
       <c r="D62" s="151"/>
       <c r="E62" s="152"/>
       <c r="F62" s="303" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G62" s="303"/>
       <c r="H62" s="303"/>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="E63" s="321"/>
       <c r="F63" s="303" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G63" s="303"/>
       <c r="H63" s="303"/>
@@ -10057,7 +10057,7 @@
       <c r="D64" s="151"/>
       <c r="E64" s="152"/>
       <c r="F64" s="303" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G64" s="303"/>
       <c r="H64" s="303"/>
@@ -10093,7 +10093,7 @@
       <c r="D65" s="151"/>
       <c r="E65" s="152"/>
       <c r="F65" s="303" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G65" s="303"/>
       <c r="H65" s="303"/>
@@ -10129,7 +10129,7 @@
       <c r="D66" s="151"/>
       <c r="E66" s="152"/>
       <c r="F66" s="303" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G66" s="303"/>
       <c r="H66" s="303"/>
@@ -10159,13 +10159,13 @@
     <row r="67" spans="1:30" ht="17.25" customHeight="1">
       <c r="A67" s="69"/>
       <c r="B67" s="319" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C67" s="320"/>
       <c r="D67" s="320"/>
       <c r="E67" s="321"/>
       <c r="F67" s="303" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G67" s="303"/>
       <c r="H67" s="303"/>
@@ -10195,13 +10195,13 @@
     <row r="68" spans="1:30" ht="17.25" customHeight="1">
       <c r="A68" s="69"/>
       <c r="B68" s="150" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C68" s="151"/>
       <c r="D68" s="151"/>
       <c r="E68" s="152"/>
       <c r="F68" s="303" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G68" s="303"/>
       <c r="H68" s="303"/>
@@ -10231,13 +10231,13 @@
     <row r="69" spans="1:30" ht="17.25" customHeight="1">
       <c r="A69" s="69"/>
       <c r="B69" s="150" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C69" s="151"/>
       <c r="D69" s="151"/>
       <c r="E69" s="152"/>
       <c r="F69" s="303" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G69" s="303"/>
       <c r="H69" s="303"/>
@@ -10273,7 +10273,7 @@
       <c r="D70" s="151"/>
       <c r="E70" s="152"/>
       <c r="F70" s="300" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G70" s="301"/>
       <c r="H70" s="301"/>
@@ -10302,7 +10302,7 @@
     </row>
     <row r="71" spans="1:30" ht="15.75" customHeight="1">
       <c r="A71" s="157" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B71" s="69"/>
       <c r="C71" s="158"/>
@@ -10598,9 +10598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14:W14"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -10614,18 +10612,18 @@
     <row r="1" spans="1:28"/>
     <row r="2" spans="1:28">
       <c r="A2" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:28"/>
     <row r="5" spans="1:28">
       <c r="A5" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -10660,7 +10658,7 @@
     </row>
     <row r="7" spans="1:28">
       <c r="B7" s="7" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -10683,69 +10681,69 @@
     </row>
     <row r="8" spans="1:28">
       <c r="B8" s="346" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C8" s="346"/>
       <c r="D8" s="346"/>
       <c r="E8" s="346"/>
       <c r="F8" s="344" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="G8" s="345"/>
       <c r="J8" s="346" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K8" s="346"/>
       <c r="L8" s="346"/>
       <c r="M8" s="347"/>
       <c r="N8" s="344" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="O8" s="345"/>
       <c r="R8" s="8"/>
     </row>
     <row r="9" spans="1:28">
       <c r="B9" s="346" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C9" s="346"/>
       <c r="D9" s="346"/>
       <c r="E9" s="346"/>
       <c r="F9" s="344" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G9" s="345"/>
       <c r="J9" s="346" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="K9" s="346"/>
       <c r="L9" s="346"/>
       <c r="M9" s="347"/>
       <c r="N9" s="344" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="O9" s="345"/>
       <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:28">
       <c r="B10" s="346" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C10" s="346"/>
       <c r="D10" s="346"/>
       <c r="E10" s="346"/>
       <c r="F10" s="344" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G10" s="345"/>
       <c r="J10" s="346" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="K10" s="346"/>
       <c r="L10" s="346"/>
       <c r="M10" s="347"/>
       <c r="N10" s="344" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O10" s="345"/>
       <c r="R10" s="8"/>
@@ -10780,33 +10778,33 @@
     </row>
     <row r="13" spans="1:28">
       <c r="B13" s="358" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C13" s="358"/>
       <c r="D13" s="358"/>
       <c r="E13" s="344" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F13" s="345"/>
       <c r="H13" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="353" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L13" s="353" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="358" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="O13" s="358"/>
       <c r="P13" s="358"/>
       <c r="Q13" s="344" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="R13" s="345"/>
       <c r="S13" s="13"/>
@@ -10814,71 +10812,71 @@
     </row>
     <row r="14" spans="1:28">
       <c r="B14" s="358" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C14" s="358"/>
       <c r="D14" s="358"/>
       <c r="E14" s="344" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F14" s="345"/>
       <c r="H14" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="353" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="L14" s="353"/>
       <c r="M14" s="11"/>
       <c r="N14" s="358" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="O14" s="358"/>
       <c r="P14" s="358"/>
       <c r="Q14" s="344" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="R14" s="345"/>
       <c r="T14" s="358" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="U14" s="358"/>
       <c r="V14" s="344" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="W14" s="345"/>
     </row>
     <row r="15" spans="1:28">
       <c r="B15" s="358" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C15" s="358"/>
       <c r="D15" s="358"/>
       <c r="E15" s="344" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F15" s="345"/>
       <c r="H15" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="353" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="L15" s="353" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="358" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="O15" s="358"/>
       <c r="P15" s="358"/>
       <c r="Q15" s="344" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="R15" s="345"/>
       <c r="S15" s="13"/>
@@ -10891,7 +10889,7 @@
     </row>
     <row r="17" spans="2:22">
       <c r="B17" s="15" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -10909,59 +10907,59 @@
     </row>
     <row r="18" spans="2:22" ht="15" customHeight="1">
       <c r="B18" s="20" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="5"/>
       <c r="E18" s="16"/>
       <c r="F18" s="351" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G18" s="352"/>
       <c r="H18" s="344" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I18" s="345"/>
       <c r="J18" s="16"/>
       <c r="K18" s="351" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L18" s="352"/>
       <c r="M18" s="344" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N18" s="345"/>
       <c r="O18" s="19"/>
     </row>
     <row r="19" spans="2:22" ht="15" customHeight="1">
       <c r="B19" s="20" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="16"/>
       <c r="F19" s="351" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G19" s="352"/>
       <c r="H19" s="344" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I19" s="345"/>
       <c r="J19" s="16"/>
       <c r="K19" s="351" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L19" s="352"/>
       <c r="M19" s="344" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N19" s="345"/>
       <c r="O19" s="19"/>
     </row>
     <row r="20" spans="2:22">
       <c r="B20" s="20" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -10979,7 +10977,7 @@
     </row>
     <row r="22" spans="2:22">
       <c r="B22" s="15" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -11004,7 +11002,7 @@
     </row>
     <row r="23" spans="2:22">
       <c r="B23" s="20" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -11012,15 +11010,15 @@
       <c r="F23" s="16"/>
       <c r="G23" s="4"/>
       <c r="H23" s="353" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="I23" s="353" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="354" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M23" s="355"/>
       <c r="N23" s="356"/>
@@ -11035,7 +11033,7 @@
     </row>
     <row r="24" spans="2:22">
       <c r="B24" s="360" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C24" s="360"/>
       <c r="D24" s="360"/>
@@ -11060,7 +11058,7 @@
     </row>
     <row r="25" spans="2:22">
       <c r="B25" s="22" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -11108,7 +11106,7 @@
     </row>
     <row r="28" spans="2:22">
       <c r="B28" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -11128,21 +11126,21 @@
     </row>
     <row r="29" spans="2:22">
       <c r="B29" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C29" s="356" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D29" s="359"/>
       <c r="E29" s="359"/>
       <c r="F29" s="357"/>
       <c r="H29" s="366" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I29" s="366"/>
       <c r="J29" s="366"/>
       <c r="K29" s="27" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L29" s="28"/>
       <c r="M29" s="27"/>
@@ -11150,7 +11148,7 @@
     </row>
     <row r="30" spans="2:22">
       <c r="B30" s="29" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
@@ -11170,7 +11168,7 @@
     </row>
     <row r="31" spans="2:22">
       <c r="B31" s="31" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
@@ -11190,7 +11188,7 @@
     </row>
     <row r="32" spans="2:22">
       <c r="B32" s="29" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31"/>
@@ -11228,7 +11226,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
@@ -11258,33 +11256,33 @@
     <row r="35" spans="1:25">
       <c r="A35" s="41"/>
       <c r="B35" s="374" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C35" s="375"/>
       <c r="D35" s="375"/>
       <c r="E35" s="375"/>
       <c r="F35" s="376"/>
       <c r="G35" s="364" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="H35" s="364"/>
       <c r="I35" s="364"/>
       <c r="J35" s="364"/>
       <c r="K35" s="364"/>
       <c r="L35" s="42" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="M35" s="371"/>
       <c r="N35" s="372"/>
       <c r="O35" s="373"/>
       <c r="P35" s="378" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="Q35" s="379"/>
       <c r="R35" s="379"/>
       <c r="S35" s="380"/>
       <c r="T35" s="361" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="U35" s="362"/>
       <c r="V35" s="362"/>
@@ -11311,13 +11309,13 @@
       <c r="N36" s="368"/>
       <c r="O36" s="369"/>
       <c r="P36" s="378" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="Q36" s="379"/>
       <c r="R36" s="379"/>
       <c r="S36" s="380"/>
       <c r="T36" s="364" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="U36" s="364"/>
       <c r="V36" s="364"/>
@@ -11328,14 +11326,14 @@
     <row r="37" spans="1:25" ht="14.4" customHeight="1">
       <c r="A37" s="41"/>
       <c r="B37" s="377" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C37" s="377"/>
       <c r="D37" s="377"/>
       <c r="E37" s="377"/>
       <c r="F37" s="377"/>
       <c r="G37" s="365" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H37" s="365"/>
       <c r="I37" s="365"/>
@@ -11346,13 +11344,13 @@
       <c r="N37" s="365"/>
       <c r="O37" s="365"/>
       <c r="P37" s="381" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="Q37" s="381"/>
       <c r="R37" s="381"/>
       <c r="S37" s="381"/>
       <c r="T37" s="370" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="U37" s="370"/>
       <c r="V37" s="370"/>
@@ -11363,11 +11361,11 @@
     <row r="38" spans="1:25" customFormat="1" ht="14.4" customHeight="1"/>
     <row r="39" spans="1:25">
       <c r="B39" s="342" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C39" s="342"/>
       <c r="D39" s="343" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E39" s="343"/>
       <c r="F39" s="343"/>
@@ -11382,10 +11380,10 @@
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="35" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="R39" s="343" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="S39" s="343"/>
       <c r="T39" s="343"/>
@@ -11421,7 +11419,7 @@
     </row>
     <row r="41" spans="1:25">
       <c r="B41" s="37" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C41" s="340"/>
       <c r="D41" s="340"/>
@@ -11430,7 +11428,7 @@
       <c r="G41" s="340"/>
       <c r="H41" s="5"/>
       <c r="I41" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J41" s="340"/>
       <c r="K41" s="340"/>
@@ -11440,7 +11438,7 @@
       <c r="O41" s="340"/>
       <c r="P41" s="5"/>
       <c r="Q41" s="4" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="R41" s="341"/>
       <c r="S41" s="341"/>
@@ -11452,7 +11450,7 @@
     </row>
     <row r="42" spans="1:25">
       <c r="B42" s="37" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C42" s="340"/>
       <c r="D42" s="340"/>
@@ -11461,7 +11459,7 @@
       <c r="G42" s="340"/>
       <c r="H42" s="5"/>
       <c r="I42" s="4" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J42" s="340"/>
       <c r="K42" s="340"/>
@@ -11471,7 +11469,7 @@
       <c r="O42" s="340"/>
       <c r="P42" s="5"/>
       <c r="Q42" s="4" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="R42" s="341"/>
       <c r="S42" s="341"/>
@@ -11483,7 +11481,7 @@
     </row>
     <row r="43" spans="1:25">
       <c r="B43" s="37" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C43" s="340"/>
       <c r="D43" s="340"/>
@@ -11492,7 +11490,7 @@
       <c r="G43" s="340"/>
       <c r="H43" s="5"/>
       <c r="I43" s="4" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="J43" s="340"/>
       <c r="K43" s="340"/>
@@ -11502,7 +11500,7 @@
       <c r="O43" s="340"/>
       <c r="P43" s="5"/>
       <c r="Q43" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="R43" s="341"/>
       <c r="S43" s="341"/>
@@ -11649,9 +11647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW1041"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:F34"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="15.6"/>
   <cols>
@@ -11687,12 +11683,12 @@
         <v>45</v>
       </c>
       <c r="B2" s="410" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="410"/>
       <c r="D2" s="410"/>
       <c r="E2" s="387" t="s">
-        <v>53</v>
+        <v>583</v>
       </c>
       <c r="F2" s="388"/>
       <c r="G2" s="388"/>
@@ -11746,7 +11742,7 @@
         <v>46</v>
       </c>
       <c r="B3" s="410" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="410"/>
       <c r="D3" s="410"/>
@@ -11883,19 +11879,19 @@
     </row>
     <row r="5" spans="1:75" ht="18" customHeight="1">
       <c r="A5" s="420" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B5" s="393" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C5" s="415" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="395" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E5" s="400" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F5" s="401"/>
       <c r="G5" s="172"/>
@@ -12047,19 +12043,19 @@
     </row>
     <row r="7" spans="1:75">
       <c r="A7" s="397" t="s">
+        <v>327</v>
+      </c>
+      <c r="B7" s="418" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" s="397" t="s">
         <v>329</v>
       </c>
-      <c r="B7" s="418" t="s">
+      <c r="D7" s="399" t="s">
         <v>330</v>
       </c>
-      <c r="C7" s="397" t="s">
-        <v>331</v>
-      </c>
-      <c r="D7" s="399" t="s">
-        <v>332</v>
-      </c>
       <c r="E7" s="413" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F7" s="414"/>
       <c r="G7" s="117"/>
@@ -12116,7 +12112,7 @@
       <c r="C8" s="397"/>
       <c r="D8" s="399"/>
       <c r="E8" s="413" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F8" s="414"/>
       <c r="G8" s="117"/>
@@ -12166,19 +12162,19 @@
     </row>
     <row r="9" spans="1:75">
       <c r="A9" s="397" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" s="398" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="397" t="s">
         <v>333</v>
       </c>
-      <c r="B9" s="398" t="s">
+      <c r="D9" s="399" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="397" t="s">
-        <v>335</v>
-      </c>
-      <c r="D9" s="399" t="s">
-        <v>336</v>
-      </c>
       <c r="E9" s="413" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F9" s="414"/>
       <c r="G9" s="117"/>
@@ -12232,7 +12228,7 @@
       <c r="C10" s="397"/>
       <c r="D10" s="399"/>
       <c r="E10" s="413" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F10" s="414"/>
       <c r="G10" s="117"/>
@@ -12286,19 +12282,19 @@
     </row>
     <row r="11" spans="1:75">
       <c r="A11" s="397" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="398" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="397" t="s">
         <v>337</v>
       </c>
-      <c r="B11" s="398" t="s">
+      <c r="D11" s="399" t="s">
         <v>338</v>
       </c>
-      <c r="C11" s="397" t="s">
-        <v>339</v>
-      </c>
-      <c r="D11" s="399" t="s">
-        <v>340</v>
-      </c>
       <c r="E11" s="413" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F11" s="414"/>
       <c r="G11" s="117"/>
@@ -12357,7 +12353,7 @@
       <c r="C12" s="397"/>
       <c r="D12" s="399"/>
       <c r="E12" s="413" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F12" s="414"/>
       <c r="G12" s="117"/>
@@ -12412,19 +12408,19 @@
     </row>
     <row r="13" spans="1:75">
       <c r="A13" s="397" t="s">
+        <v>339</v>
+      </c>
+      <c r="B13" s="398" t="s">
+        <v>340</v>
+      </c>
+      <c r="C13" s="397" t="s">
         <v>341</v>
       </c>
-      <c r="B13" s="398" t="s">
+      <c r="D13" s="399" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="397" t="s">
-        <v>343</v>
-      </c>
-      <c r="D13" s="399" t="s">
-        <v>344</v>
-      </c>
       <c r="E13" s="413" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F13" s="414"/>
       <c r="G13" s="117"/>
@@ -12483,7 +12479,7 @@
       <c r="C14" s="397"/>
       <c r="D14" s="399"/>
       <c r="E14" s="413" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F14" s="414"/>
       <c r="G14" s="117"/>
@@ -12538,19 +12534,19 @@
     </row>
     <row r="15" spans="1:75">
       <c r="A15" s="397" t="s">
+        <v>343</v>
+      </c>
+      <c r="B15" s="398" t="s">
+        <v>344</v>
+      </c>
+      <c r="C15" s="397" t="s">
         <v>345</v>
       </c>
-      <c r="B15" s="398" t="s">
+      <c r="D15" s="399" t="s">
         <v>346</v>
       </c>
-      <c r="C15" s="397" t="s">
-        <v>347</v>
-      </c>
-      <c r="D15" s="399" t="s">
-        <v>348</v>
-      </c>
       <c r="E15" s="413" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F15" s="414"/>
       <c r="G15" s="117"/>
@@ -12609,7 +12605,7 @@
       <c r="C16" s="397"/>
       <c r="D16" s="399"/>
       <c r="E16" s="413" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F16" s="414"/>
       <c r="G16" s="117"/>
@@ -12659,19 +12655,19 @@
     </row>
     <row r="17" spans="1:75">
       <c r="A17" s="397" t="s">
+        <v>347</v>
+      </c>
+      <c r="B17" s="398" t="s">
+        <v>348</v>
+      </c>
+      <c r="C17" s="397" t="s">
         <v>349</v>
       </c>
-      <c r="B17" s="398" t="s">
+      <c r="D17" s="399" t="s">
         <v>350</v>
       </c>
-      <c r="C17" s="397" t="s">
-        <v>351</v>
-      </c>
-      <c r="D17" s="399" t="s">
-        <v>352</v>
-      </c>
       <c r="E17" s="413" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F17" s="414"/>
       <c r="G17" s="117"/>
@@ -12725,7 +12721,7 @@
       <c r="C18" s="397"/>
       <c r="D18" s="399"/>
       <c r="E18" s="413" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F18" s="414"/>
       <c r="G18" s="117"/>
@@ -12783,19 +12779,19 @@
     </row>
     <row r="19" spans="1:75">
       <c r="A19" s="397" t="s">
+        <v>351</v>
+      </c>
+      <c r="B19" s="398" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" s="397" t="s">
         <v>353</v>
       </c>
-      <c r="B19" s="398" t="s">
+      <c r="D19" s="399" t="s">
         <v>354</v>
       </c>
-      <c r="C19" s="397" t="s">
-        <v>355</v>
-      </c>
-      <c r="D19" s="399" t="s">
-        <v>356</v>
-      </c>
       <c r="E19" s="413" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F19" s="414"/>
       <c r="G19" s="117"/>
@@ -12849,7 +12845,7 @@
       <c r="C20" s="397"/>
       <c r="D20" s="399"/>
       <c r="E20" s="413" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F20" s="414"/>
       <c r="G20" s="117"/>
@@ -12899,19 +12895,19 @@
     </row>
     <row r="21" spans="1:75">
       <c r="A21" s="397" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" s="398" t="s">
+        <v>356</v>
+      </c>
+      <c r="C21" s="397" t="s">
         <v>357</v>
       </c>
-      <c r="B21" s="398" t="s">
+      <c r="D21" s="399" t="s">
         <v>358</v>
       </c>
-      <c r="C21" s="397" t="s">
-        <v>359</v>
-      </c>
-      <c r="D21" s="399" t="s">
-        <v>360</v>
-      </c>
       <c r="E21" s="413" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F21" s="414"/>
       <c r="G21" s="117"/>
@@ -12965,7 +12961,7 @@
       <c r="C22" s="397"/>
       <c r="D22" s="399"/>
       <c r="E22" s="413" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F22" s="414"/>
       <c r="G22" s="117"/>
@@ -13015,19 +13011,19 @@
     </row>
     <row r="23" spans="1:75">
       <c r="A23" s="397" t="s">
+        <v>359</v>
+      </c>
+      <c r="B23" s="398" t="s">
+        <v>360</v>
+      </c>
+      <c r="C23" s="397" t="s">
         <v>361</v>
       </c>
-      <c r="B23" s="398" t="s">
+      <c r="D23" s="399" t="s">
         <v>362</v>
       </c>
-      <c r="C23" s="397" t="s">
-        <v>363</v>
-      </c>
-      <c r="D23" s="399" t="s">
-        <v>364</v>
-      </c>
       <c r="E23" s="413" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F23" s="414"/>
       <c r="G23" s="117"/>
@@ -13081,7 +13077,7 @@
       <c r="C24" s="397"/>
       <c r="D24" s="399"/>
       <c r="E24" s="413" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F24" s="414"/>
       <c r="G24" s="117"/>
@@ -13131,19 +13127,19 @@
     </row>
     <row r="25" spans="1:75">
       <c r="A25" s="397" t="s">
+        <v>363</v>
+      </c>
+      <c r="B25" s="398" t="s">
+        <v>364</v>
+      </c>
+      <c r="C25" s="397" t="s">
         <v>365</v>
       </c>
-      <c r="B25" s="398" t="s">
+      <c r="D25" s="399" t="s">
         <v>366</v>
       </c>
-      <c r="C25" s="397" t="s">
-        <v>367</v>
-      </c>
-      <c r="D25" s="399" t="s">
-        <v>368</v>
-      </c>
       <c r="E25" s="413" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F25" s="414"/>
       <c r="G25" s="117"/>
@@ -13197,7 +13193,7 @@
       <c r="C26" s="397"/>
       <c r="D26" s="399"/>
       <c r="E26" s="413" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F26" s="414"/>
       <c r="G26" s="117"/>
@@ -13247,19 +13243,19 @@
     </row>
     <row r="27" spans="1:75">
       <c r="A27" s="397" t="s">
+        <v>367</v>
+      </c>
+      <c r="B27" s="398" t="s">
+        <v>368</v>
+      </c>
+      <c r="C27" s="397" t="s">
         <v>369</v>
       </c>
-      <c r="B27" s="398" t="s">
+      <c r="D27" s="399" t="s">
         <v>370</v>
       </c>
-      <c r="C27" s="397" t="s">
-        <v>371</v>
-      </c>
-      <c r="D27" s="399" t="s">
-        <v>372</v>
-      </c>
       <c r="E27" s="413" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F27" s="414"/>
       <c r="G27" s="117"/>
@@ -13313,7 +13309,7 @@
       <c r="C28" s="397"/>
       <c r="D28" s="399"/>
       <c r="E28" s="413" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F28" s="414"/>
       <c r="G28" s="117"/>
@@ -13363,19 +13359,19 @@
     </row>
     <row r="29" spans="1:75">
       <c r="A29" s="397" t="s">
+        <v>371</v>
+      </c>
+      <c r="B29" s="398" t="s">
+        <v>372</v>
+      </c>
+      <c r="C29" s="397" t="s">
         <v>373</v>
       </c>
-      <c r="B29" s="398" t="s">
+      <c r="D29" s="399" t="s">
         <v>374</v>
       </c>
-      <c r="C29" s="397" t="s">
-        <v>375</v>
-      </c>
-      <c r="D29" s="399" t="s">
-        <v>376</v>
-      </c>
       <c r="E29" s="413" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F29" s="414"/>
       <c r="G29" s="117"/>
@@ -13429,7 +13425,7 @@
       <c r="C30" s="397"/>
       <c r="D30" s="399"/>
       <c r="E30" s="413" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F30" s="414"/>
       <c r="G30" s="117"/>
@@ -13479,19 +13475,19 @@
     </row>
     <row r="31" spans="1:75">
       <c r="A31" s="397" t="s">
+        <v>375</v>
+      </c>
+      <c r="B31" s="398" t="s">
+        <v>376</v>
+      </c>
+      <c r="C31" s="397" t="s">
         <v>377</v>
       </c>
-      <c r="B31" s="398" t="s">
+      <c r="D31" s="399" t="s">
         <v>378</v>
       </c>
-      <c r="C31" s="397" t="s">
-        <v>379</v>
-      </c>
-      <c r="D31" s="399" t="s">
-        <v>380</v>
-      </c>
       <c r="E31" s="413" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F31" s="414"/>
       <c r="G31" s="117"/>
@@ -13545,7 +13541,7 @@
       <c r="C32" s="397"/>
       <c r="D32" s="399"/>
       <c r="E32" s="413" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F32" s="414"/>
       <c r="G32" s="117"/>
@@ -13595,19 +13591,19 @@
     </row>
     <row r="33" spans="1:75">
       <c r="A33" s="397" t="s">
+        <v>379</v>
+      </c>
+      <c r="B33" s="398" t="s">
+        <v>380</v>
+      </c>
+      <c r="C33" s="397" t="s">
         <v>381</v>
       </c>
-      <c r="B33" s="398" t="s">
+      <c r="D33" s="399" t="s">
         <v>382</v>
       </c>
-      <c r="C33" s="397" t="s">
-        <v>383</v>
-      </c>
-      <c r="D33" s="399" t="s">
-        <v>384</v>
-      </c>
       <c r="E33" s="413" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F33" s="414"/>
       <c r="G33" s="117"/>
@@ -13661,7 +13657,7 @@
       <c r="C34" s="397"/>
       <c r="D34" s="399"/>
       <c r="E34" s="413" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F34" s="414"/>
       <c r="G34" s="117"/>
@@ -13711,19 +13707,19 @@
     </row>
     <row r="35" spans="1:75">
       <c r="A35" s="397" t="s">
+        <v>383</v>
+      </c>
+      <c r="B35" s="398" t="s">
+        <v>384</v>
+      </c>
+      <c r="C35" s="397" t="s">
         <v>385</v>
       </c>
-      <c r="B35" s="398" t="s">
+      <c r="D35" s="399" t="s">
         <v>386</v>
       </c>
-      <c r="C35" s="397" t="s">
-        <v>387</v>
-      </c>
-      <c r="D35" s="399" t="s">
-        <v>388</v>
-      </c>
       <c r="E35" s="413" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F35" s="414"/>
       <c r="G35" s="117"/>
@@ -13777,7 +13773,7 @@
       <c r="C36" s="397"/>
       <c r="D36" s="399"/>
       <c r="E36" s="413" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F36" s="414"/>
       <c r="G36" s="117"/>
@@ -13827,19 +13823,19 @@
     </row>
     <row r="37" spans="1:75">
       <c r="A37" s="397" t="s">
+        <v>387</v>
+      </c>
+      <c r="B37" s="398" t="s">
+        <v>388</v>
+      </c>
+      <c r="C37" s="397" t="s">
         <v>389</v>
       </c>
-      <c r="B37" s="398" t="s">
+      <c r="D37" s="399" t="s">
         <v>390</v>
       </c>
-      <c r="C37" s="397" t="s">
-        <v>391</v>
-      </c>
-      <c r="D37" s="399" t="s">
-        <v>392</v>
-      </c>
       <c r="E37" s="413" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F37" s="414"/>
       <c r="G37" s="117"/>
@@ -13893,7 +13889,7 @@
       <c r="C38" s="397"/>
       <c r="D38" s="399"/>
       <c r="E38" s="413" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F38" s="414"/>
       <c r="G38" s="117"/>
@@ -13943,19 +13939,19 @@
     </row>
     <row r="39" spans="1:75">
       <c r="A39" s="397" t="s">
+        <v>391</v>
+      </c>
+      <c r="B39" s="398" t="s">
+        <v>392</v>
+      </c>
+      <c r="C39" s="397" t="s">
         <v>393</v>
       </c>
-      <c r="B39" s="398" t="s">
+      <c r="D39" s="399" t="s">
         <v>394</v>
       </c>
-      <c r="C39" s="397" t="s">
-        <v>395</v>
-      </c>
-      <c r="D39" s="399" t="s">
-        <v>396</v>
-      </c>
       <c r="E39" s="413" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F39" s="414"/>
       <c r="G39" s="117"/>
@@ -14009,7 +14005,7 @@
       <c r="C40" s="397"/>
       <c r="D40" s="399"/>
       <c r="E40" s="413" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F40" s="414"/>
       <c r="G40" s="117"/>
@@ -14083,7 +14079,7 @@
     </row>
     <row r="41" spans="1:75" ht="45.75" customHeight="1">
       <c r="A41" s="384" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B41" s="385"/>
       <c r="C41" s="385"/>
@@ -14091,7 +14087,7 @@
       <c r="E41" s="385"/>
       <c r="F41" s="386"/>
       <c r="G41" s="382" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="H41" s="383"/>
       <c r="I41" s="117"/>
@@ -14162,15 +14158,15 @@
     </row>
     <row r="42" spans="1:75" s="195" customFormat="1" ht="15" customHeight="1">
       <c r="A42" s="425" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B42" s="426"/>
       <c r="C42" s="429" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D42" s="430"/>
       <c r="E42" s="413" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F42" s="414"/>
       <c r="G42" s="117"/>
@@ -14247,7 +14243,7 @@
       <c r="C43" s="431"/>
       <c r="D43" s="432"/>
       <c r="E43" s="423" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F43" s="424"/>
       <c r="G43" s="117"/>
@@ -14322,11 +14318,11 @@
       <c r="A44" s="425"/>
       <c r="B44" s="426"/>
       <c r="C44" s="433" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D44" s="434"/>
       <c r="E44" s="413" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F44" s="414"/>
       <c r="G44" s="117"/>
@@ -14403,7 +14399,7 @@
       <c r="C45" s="431"/>
       <c r="D45" s="432"/>
       <c r="E45" s="423" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F45" s="424"/>
       <c r="G45" s="117"/>
@@ -14478,11 +14474,11 @@
       <c r="A46" s="425"/>
       <c r="B46" s="426"/>
       <c r="C46" s="433" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D46" s="434"/>
       <c r="E46" s="413" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F46" s="414"/>
       <c r="G46" s="117"/>
@@ -14559,7 +14555,7 @@
       <c r="C47" s="431"/>
       <c r="D47" s="432"/>
       <c r="E47" s="423" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F47" s="424"/>
       <c r="G47" s="117"/>
@@ -14634,11 +14630,11 @@
       <c r="A48" s="425"/>
       <c r="B48" s="426"/>
       <c r="C48" s="433" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D48" s="434"/>
       <c r="E48" s="413" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F48" s="414"/>
       <c r="G48" s="117"/>
@@ -14715,7 +14711,7 @@
       <c r="C49" s="431"/>
       <c r="D49" s="432"/>
       <c r="E49" s="423" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F49" s="424"/>
       <c r="G49" s="117"/>
@@ -14790,11 +14786,11 @@
       <c r="A50" s="425"/>
       <c r="B50" s="426"/>
       <c r="C50" s="433" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D50" s="434"/>
       <c r="E50" s="413" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F50" s="414"/>
       <c r="G50" s="117"/>
@@ -14871,7 +14867,7 @@
       <c r="C51" s="431"/>
       <c r="D51" s="432"/>
       <c r="E51" s="423" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F51" s="424"/>
       <c r="G51" s="117"/>
@@ -14946,11 +14942,11 @@
       <c r="A52" s="425"/>
       <c r="B52" s="426"/>
       <c r="C52" s="433" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D52" s="434"/>
       <c r="E52" s="413" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F52" s="414"/>
       <c r="G52" s="117"/>
@@ -15027,7 +15023,7 @@
       <c r="C53" s="431"/>
       <c r="D53" s="432"/>
       <c r="E53" s="423" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F53" s="424"/>
       <c r="G53" s="117"/>
@@ -15102,11 +15098,11 @@
       <c r="A54" s="425"/>
       <c r="B54" s="426"/>
       <c r="C54" s="433" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D54" s="434"/>
       <c r="E54" s="413" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F54" s="414"/>
       <c r="G54" s="117"/>
@@ -15183,7 +15179,7 @@
       <c r="C55" s="431"/>
       <c r="D55" s="432"/>
       <c r="E55" s="423" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F55" s="424"/>
       <c r="G55" s="117"/>
@@ -15258,11 +15254,11 @@
       <c r="A56" s="425"/>
       <c r="B56" s="426"/>
       <c r="C56" s="433" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D56" s="434"/>
       <c r="E56" s="423" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F56" s="424"/>
       <c r="G56" s="117"/>
@@ -15339,7 +15335,7 @@
       <c r="C57" s="431"/>
       <c r="D57" s="432"/>
       <c r="E57" s="423" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F57" s="424"/>
       <c r="G57" s="117"/>
@@ -15414,11 +15410,11 @@
       <c r="A58" s="425"/>
       <c r="B58" s="426"/>
       <c r="C58" s="433" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D58" s="434"/>
       <c r="E58" s="413" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F58" s="414"/>
       <c r="G58" s="117"/>
@@ -15495,7 +15491,7 @@
       <c r="C59" s="431"/>
       <c r="D59" s="432"/>
       <c r="E59" s="423" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F59" s="424"/>
       <c r="G59" s="117"/>
@@ -15570,11 +15566,11 @@
       <c r="A60" s="425"/>
       <c r="B60" s="426"/>
       <c r="C60" s="433" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D60" s="434"/>
       <c r="E60" s="413" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F60" s="414"/>
       <c r="G60" s="117"/>
@@ -15651,7 +15647,7 @@
       <c r="C61" s="431"/>
       <c r="D61" s="432"/>
       <c r="E61" s="423" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F61" s="424"/>
       <c r="G61" s="117"/>
@@ -15726,11 +15722,11 @@
       <c r="A62" s="425"/>
       <c r="B62" s="426"/>
       <c r="C62" s="433" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D62" s="434"/>
       <c r="E62" s="413" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F62" s="414"/>
       <c r="G62" s="117"/>
@@ -15807,7 +15803,7 @@
       <c r="C63" s="431"/>
       <c r="D63" s="432"/>
       <c r="E63" s="423" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F63" s="424"/>
       <c r="G63" s="117"/>
@@ -15882,11 +15878,11 @@
       <c r="A64" s="425"/>
       <c r="B64" s="426"/>
       <c r="C64" s="433" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D64" s="434"/>
       <c r="E64" s="413" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F64" s="414"/>
       <c r="G64" s="117"/>
@@ -15963,7 +15959,7 @@
       <c r="C65" s="431"/>
       <c r="D65" s="432"/>
       <c r="E65" s="423" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F65" s="424"/>
       <c r="G65" s="117"/>
@@ -16038,11 +16034,11 @@
       <c r="A66" s="425"/>
       <c r="B66" s="426"/>
       <c r="C66" s="433" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D66" s="434"/>
       <c r="E66" s="413" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F66" s="414"/>
       <c r="G66" s="117"/>
@@ -16119,7 +16115,7 @@
       <c r="C67" s="431"/>
       <c r="D67" s="432"/>
       <c r="E67" s="423" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F67" s="424"/>
       <c r="G67" s="117"/>
@@ -16194,11 +16190,11 @@
       <c r="A68" s="425"/>
       <c r="B68" s="426"/>
       <c r="C68" s="433" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D68" s="434"/>
       <c r="E68" s="413" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F68" s="414"/>
       <c r="G68" s="117"/>
@@ -16277,7 +16273,7 @@
       <c r="C69" s="431"/>
       <c r="D69" s="432"/>
       <c r="E69" s="423" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F69" s="424"/>
       <c r="G69" s="117"/>
@@ -16354,11 +16350,11 @@
       <c r="A70" s="425"/>
       <c r="B70" s="426"/>
       <c r="C70" s="433" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D70" s="434"/>
       <c r="E70" s="413" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F70" s="414"/>
       <c r="G70" s="117"/>
@@ -16437,7 +16433,7 @@
       <c r="C71" s="431"/>
       <c r="D71" s="432"/>
       <c r="E71" s="423" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F71" s="424"/>
       <c r="G71" s="117"/>
@@ -16757,7 +16753,7 @@
       </c>
       <c r="D75" s="409"/>
       <c r="E75" s="423" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F75" s="424"/>
       <c r="G75" s="117"/>
@@ -16838,7 +16834,7 @@
       </c>
       <c r="D76" s="409"/>
       <c r="E76" s="423" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F76" s="424"/>
       <c r="G76" s="117"/>
@@ -16919,7 +16915,7 @@
       </c>
       <c r="D77" s="409"/>
       <c r="E77" s="423" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F77" s="424"/>
       <c r="G77" s="117"/>
@@ -16996,11 +16992,11 @@
       <c r="A78" s="451"/>
       <c r="B78" s="452"/>
       <c r="C78" s="408" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D78" s="409"/>
       <c r="E78" s="423" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F78" s="424"/>
       <c r="G78" s="117"/>
@@ -17081,7 +17077,7 @@
       </c>
       <c r="D79" s="409"/>
       <c r="E79" s="423" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F79" s="424"/>
       <c r="G79" s="117"/>
@@ -17162,7 +17158,7 @@
       <c r="C80" s="454"/>
       <c r="D80" s="454"/>
       <c r="E80" s="453" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F80" s="424"/>
       <c r="G80" s="117"/>
@@ -17243,7 +17239,7 @@
       <c r="C81" s="454"/>
       <c r="D81" s="454"/>
       <c r="E81" s="453" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F81" s="424"/>
       <c r="G81" s="117"/>
@@ -17359,11 +17355,11 @@
     <row r="83" spans="1:75" ht="14.1" customHeight="1" thickBot="1">
       <c r="A83" s="205"/>
       <c r="B83" s="214" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C83" s="213"/>
       <c r="D83" s="448" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E83" s="448"/>
       <c r="F83" s="206"/>
@@ -17403,11 +17399,11 @@
     <row r="84" spans="1:75" ht="13.8" customHeight="1" thickBot="1">
       <c r="A84" s="205"/>
       <c r="B84" s="215" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C84" s="213"/>
       <c r="D84" s="448" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E84" s="448"/>
       <c r="F84" s="206"/>

</xml_diff>